<commit_message>
vault backup: 2025-04-07 03:23:02
</commit_message>
<xml_diff>
--- a/Economics/Dissertation/Dissertation Presentation Sheets.xlsx
+++ b/Economics/Dissertation/Dissertation Presentation Sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Economics\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C6339CC-9174-464D-9665-BC7746C877CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8684DF-58C8-4995-BA13-EF66628B5BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="12" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="12" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Median Wage and Productivity" sheetId="1" r:id="rId1"/>
@@ -1606,7 +1606,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="24">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1651,7 +1651,6 @@
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="47">
     <cellStyle name="20% - Accent1" xfId="18" builtinId="30" customBuiltin="1"/>
@@ -36345,8 +36344,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9870522-93E5-4B17-AD12-5520AD3B40E6}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="G41" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="W15" sqref="W15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36373,10 +36372,9 @@
       <c r="F1" s="22" t="s">
         <v>313</v>
       </c>
-      <c r="G1" s="24" t="s">
+      <c r="G1" s="22" t="s">
         <v>315</v>
       </c>
-      <c r="H1" s="24"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
@@ -36591,7 +36589,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <f t="shared" ref="A11:A20" si="1">A10+10</f>
+        <f t="shared" ref="A11:A17" si="1">A10+10</f>
         <v>30</v>
       </c>
       <c r="B11">

</xml_diff>

<commit_message>
vault backup: 2025-05-03 03:54:17
</commit_message>
<xml_diff>
--- a/Economics/Dissertation/Dissertation Presentation Sheets.xlsx
+++ b/Economics/Dissertation/Dissertation Presentation Sheets.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28526"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Economics\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CC8684DF-58C8-4995-BA13-EF66628B5BA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7AC17357-3F55-4E5E-B233-5DCAEC9A73EE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="10" activeTab="12" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Median Wage and Productivity" sheetId="1" r:id="rId1"/>
@@ -26,12 +26,13 @@
     <sheet name="Productivity Measures" sheetId="10" r:id="rId11"/>
     <sheet name="Labour Share of Income" sheetId="16" r:id="rId12"/>
     <sheet name="Prelim Regression Results" sheetId="17" r:id="rId13"/>
+    <sheet name="Real Regression Results" sheetId="18" r:id="rId14"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7" hidden="1">'GDP Deflator Weights'!$O$3:$P$24</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="9" hidden="1">'Output Price Deflators'!$F$1:$I$94</definedName>
   </definedNames>
-  <calcPr calcId="191029"/>
+  <calcPr calcId="191029" calcOnSave="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -52,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="541" uniqueCount="322">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="547" uniqueCount="327">
   <si>
     <t>Year</t>
   </si>
@@ -1022,6 +1023,21 @@
   <si>
     <t>Median</t>
   </si>
+  <si>
+    <t>Prod coeff.</t>
+  </si>
+  <si>
+    <t>Error Bar</t>
+  </si>
+  <si>
+    <t>95% Confidence</t>
+  </si>
+  <si>
+    <t>A1</t>
+  </si>
+  <si>
+    <t>A2</t>
+  </si>
 </sst>
 </file>
 
@@ -1210,7 +1226,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="37">
+  <fills count="38">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1414,6 +1430,12 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="12">
     <border>
@@ -1606,7 +1628,7 @@
       <protection locked="0"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="24">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1648,7 +1670,12 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
   </cellXfs>
@@ -12663,6 +12690,1377 @@
     </a:ln>
     <a:effectLst/>
   </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr/>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB"/>
+              <a:t>Wage-productivity coefficients</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Real Regression Results'!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Prod coeff.</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Real Regression Results'!$F$2:$F$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.61709999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.6371</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.71250000000000013</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.78959999999999986</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.78200000000000003</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Real Regression Results'!$F$2:$F$6</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="5"/>
+                  <c:pt idx="0">
+                    <c:v>0.61709999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.6371</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.71250000000000013</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.78959999999999986</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.78200000000000003</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$A$2:$A$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>25</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>75</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$B$2:$B$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>0.97199999999999998</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0486</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.1299999999999999</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2154</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.335</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-907B-4A4B-A6A8-6CBBA6430998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="15875" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$G$2:$G$6</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="5"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-907B-4A4B-A6A8-6CBBA6430998}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="832559295"/>
+        <c:axId val="832558335"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="832559295"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0"/>
+                  <a:t>Wage Percentile</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="832558335"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="832558335"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" b="0"/>
+                  <a:t>Productivity Coefficient</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="832559295"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Wage-productivity coefficients</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Real Regression Results'!$F$18:$F$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.48740000000000006</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.36119999999999997</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Real Regression Results'!$F$18:$F$19</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="2"/>
+                  <c:pt idx="0">
+                    <c:v>0.48740000000000006</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.36119999999999997</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:noFill/>
+              <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:round/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:errBars>
+          <c:cat>
+            <c:strRef>
+              <c:f>'Real Regression Results'!$A$18:$A$19</c:f>
+              <c:strCache>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>A1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>A2</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$B$18:$B$19</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="2"/>
+                <c:pt idx="0">
+                  <c:v>1.1759999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.361</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-B736-4A00-BE1E-DF91D4FDD4F7}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="52229775"/>
+        <c:axId val="52226895"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="52229775"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Specification</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52226895"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="52226895"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Productivity Coefficient</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="52229775"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart22.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000"/>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Wage-productivity coefficients</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="6"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Real Regression Results'!$F$8:$F$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>0.43969999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.3708999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3647999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.38510000000000011</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.39890000000000003</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.40470000000000006</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.41030000000000011</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.41449999999999987</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.42079999999999984</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Real Regression Results'!$F$8:$F$16</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>0.43969999999999998</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.3708999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.3647999999999999</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.38510000000000011</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.39890000000000003</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.40470000000000006</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.41030000000000011</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.41449999999999987</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.42079999999999984</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+          </c:errBars>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$A$8:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$B$8:$B$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.82079999999999997</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77680000000000005</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.9103</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.96479999999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.98399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.0685</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1698999999999999</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2255</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3018000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-7824-447B-A8F8-D8541DEDA924}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$A$8:$A$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>30</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>40</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>50</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>60</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>70</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>80</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>90</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real Regression Results'!$G$8:$G$16</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-7824-447B-A8F8-D8541DEDA924}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="970994943"/>
+        <c:axId val="970995423"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="970994943"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0"/>
+                  <a:t>Wage Percentile</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="970995423"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="970995423"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0"/>
+                  <a:t>Productivity Coefficient</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="970994943"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
   <c:txPr>
     <a:bodyPr/>
     <a:lstStyle/>
@@ -21481,6 +22879,46 @@
 </file>
 
 <file path=xl/charts/colors16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -25448,6 +26886,522 @@
 </file>
 
 <file path=xl/charts/style16.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style17.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -30405,6 +32359,125 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing13.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>19</xdr:row>
+      <xdr:rowOff>180975</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{29578768-C66B-4F40-85AF-794D83AA54EE}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>612912</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>8282</xdr:colOff>
+      <xdr:row>61</xdr:row>
+      <xdr:rowOff>165652</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="11" name="Chart 10">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8EB2576D-125E-46D0-8C88-7A664E4BE7F7}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="12" name="Chart 11">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0E4F0C6B-83D3-4A14-8EFE-8157C98D817A}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -31192,7 +33265,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{34019E1C-637C-4A65-AF2C-5C3EB48F59C7}">
   <dimension ref="A1:X55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+    <sheetView topLeftCell="A7" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B9" sqref="B9:X9"/>
     </sheetView>
   </sheetViews>
@@ -36344,8 +38417,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F9870522-93E5-4B17-AD12-5520AD3B40E6}">
   <dimension ref="A1:I29"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="W15" sqref="W15"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -36365,10 +38438,10 @@
       <c r="C1" s="22" t="s">
         <v>311</v>
       </c>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="25" t="s">
         <v>312</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="25"/>
       <c r="F1" s="22" t="s">
         <v>313</v>
       </c>
@@ -37118,6 +39191,438 @@
       </c>
       <c r="I29">
         <v>0</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="D1:E1"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5295978E-5DD8-48C7-99E5-01F2CBE31AC6}">
+  <dimension ref="A1:G19"/>
+  <sheetViews>
+    <sheetView topLeftCell="A31" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="G26" sqref="G26"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="11.28515625" customWidth="1"/>
+    <col min="3" max="3" width="10.85546875" customWidth="1"/>
+    <col min="4" max="4" width="11.140625" customWidth="1"/>
+    <col min="5" max="5" width="10" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" s="24" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B1" s="24" t="s">
+        <v>322</v>
+      </c>
+      <c r="C1" s="24" t="s">
+        <v>311</v>
+      </c>
+      <c r="D1" s="26" t="s">
+        <v>324</v>
+      </c>
+      <c r="E1" s="26"/>
+      <c r="F1" s="24" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" s="23">
+        <v>10</v>
+      </c>
+      <c r="B2">
+        <v>0.97199999999999998</v>
+      </c>
+      <c r="C2">
+        <v>0.30080000000000001</v>
+      </c>
+      <c r="D2">
+        <v>0.35470000000000002</v>
+      </c>
+      <c r="E2">
+        <v>1.5891</v>
+      </c>
+      <c r="F2">
+        <f>E2-B2</f>
+        <v>0.61709999999999998</v>
+      </c>
+      <c r="G2">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" s="23">
+        <v>25</v>
+      </c>
+      <c r="B3">
+        <v>1.0486</v>
+      </c>
+      <c r="C3">
+        <v>0.3105</v>
+      </c>
+      <c r="D3">
+        <v>0.41149999999999998</v>
+      </c>
+      <c r="E3">
+        <v>1.6857</v>
+      </c>
+      <c r="F3">
+        <f t="shared" ref="F3:F6" si="0">E3-B3</f>
+        <v>0.6371</v>
+      </c>
+      <c r="G3">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" s="23">
+        <v>50</v>
+      </c>
+      <c r="B4">
+        <v>1.1299999999999999</v>
+      </c>
+      <c r="C4">
+        <v>0.3473</v>
+      </c>
+      <c r="D4">
+        <v>0.41720000000000002</v>
+      </c>
+      <c r="E4">
+        <v>1.8425</v>
+      </c>
+      <c r="F4">
+        <f t="shared" si="0"/>
+        <v>0.71250000000000013</v>
+      </c>
+      <c r="G4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" s="23">
+        <v>75</v>
+      </c>
+      <c r="B5">
+        <v>1.2154</v>
+      </c>
+      <c r="C5">
+        <v>0.38479999999999998</v>
+      </c>
+      <c r="D5">
+        <v>0.4259</v>
+      </c>
+      <c r="E5">
+        <v>2.0049999999999999</v>
+      </c>
+      <c r="F5">
+        <f t="shared" si="0"/>
+        <v>0.78959999999999986</v>
+      </c>
+      <c r="G5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A6" s="23">
+        <v>90</v>
+      </c>
+      <c r="B6">
+        <v>1.335</v>
+      </c>
+      <c r="C6">
+        <v>0.38109999999999999</v>
+      </c>
+      <c r="D6">
+        <v>0.55300000000000005</v>
+      </c>
+      <c r="E6">
+        <v>2.117</v>
+      </c>
+      <c r="F6">
+        <f t="shared" si="0"/>
+        <v>0.78200000000000003</v>
+      </c>
+      <c r="G6">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A8" s="23">
+        <v>10</v>
+      </c>
+      <c r="B8">
+        <v>0.82079999999999997</v>
+      </c>
+      <c r="C8">
+        <v>0.20930000000000001</v>
+      </c>
+      <c r="D8">
+        <v>0.38109999999999999</v>
+      </c>
+      <c r="E8">
+        <v>1.2605</v>
+      </c>
+      <c r="F8">
+        <f>E8-B8</f>
+        <v>0.43969999999999998</v>
+      </c>
+      <c r="G8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="23">
+        <f>A8+10</f>
+        <v>20</v>
+      </c>
+      <c r="B9">
+        <v>0.77680000000000005</v>
+      </c>
+      <c r="C9">
+        <v>0.17649999999999999</v>
+      </c>
+      <c r="D9">
+        <v>0.40589999999999998</v>
+      </c>
+      <c r="E9">
+        <v>1.1476999999999999</v>
+      </c>
+      <c r="F9">
+        <f t="shared" ref="F9:F16" si="1">E9-B9</f>
+        <v>0.3708999999999999</v>
+      </c>
+      <c r="G9">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="23">
+        <f t="shared" ref="A10:A16" si="2">A9+10</f>
+        <v>30</v>
+      </c>
+      <c r="B10">
+        <v>0.9103</v>
+      </c>
+      <c r="C10">
+        <v>0.1736</v>
+      </c>
+      <c r="D10">
+        <v>0.54549999999999998</v>
+      </c>
+      <c r="E10">
+        <v>1.2750999999999999</v>
+      </c>
+      <c r="F10">
+        <f t="shared" si="1"/>
+        <v>0.3647999999999999</v>
+      </c>
+      <c r="G10">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" s="23">
+        <f t="shared" si="2"/>
+        <v>40</v>
+      </c>
+      <c r="B11">
+        <v>0.96479999999999999</v>
+      </c>
+      <c r="C11">
+        <v>0.18329999999999999</v>
+      </c>
+      <c r="D11">
+        <v>0.57969999999999999</v>
+      </c>
+      <c r="E11">
+        <v>1.3499000000000001</v>
+      </c>
+      <c r="F11">
+        <f t="shared" si="1"/>
+        <v>0.38510000000000011</v>
+      </c>
+      <c r="G11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="23">
+        <f t="shared" si="2"/>
+        <v>50</v>
+      </c>
+      <c r="B12">
+        <v>0.98399999999999999</v>
+      </c>
+      <c r="C12">
+        <v>0.1898</v>
+      </c>
+      <c r="D12">
+        <v>0.58520000000000005</v>
+      </c>
+      <c r="E12">
+        <v>1.3829</v>
+      </c>
+      <c r="F12">
+        <f t="shared" si="1"/>
+        <v>0.39890000000000003</v>
+      </c>
+      <c r="G12">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="23">
+        <f t="shared" si="2"/>
+        <v>60</v>
+      </c>
+      <c r="B13">
+        <v>1.0685</v>
+      </c>
+      <c r="C13">
+        <v>0.19259999999999999</v>
+      </c>
+      <c r="D13">
+        <v>0.66390000000000005</v>
+      </c>
+      <c r="E13">
+        <v>1.4732000000000001</v>
+      </c>
+      <c r="F13">
+        <f t="shared" si="1"/>
+        <v>0.40470000000000006</v>
+      </c>
+      <c r="G13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" s="23">
+        <f t="shared" si="2"/>
+        <v>70</v>
+      </c>
+      <c r="B14">
+        <v>1.1698999999999999</v>
+      </c>
+      <c r="C14">
+        <v>0.1953</v>
+      </c>
+      <c r="D14">
+        <v>0.75949999999999995</v>
+      </c>
+      <c r="E14">
+        <v>1.5802</v>
+      </c>
+      <c r="F14">
+        <f t="shared" si="1"/>
+        <v>0.41030000000000011</v>
+      </c>
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="23">
+        <f t="shared" si="2"/>
+        <v>80</v>
+      </c>
+      <c r="B15">
+        <v>1.2255</v>
+      </c>
+      <c r="C15">
+        <v>0.1973</v>
+      </c>
+      <c r="D15">
+        <v>0.81089999999999995</v>
+      </c>
+      <c r="E15">
+        <v>1.64</v>
+      </c>
+      <c r="F15">
+        <f t="shared" si="1"/>
+        <v>0.41449999999999987</v>
+      </c>
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="23">
+        <f t="shared" si="2"/>
+        <v>90</v>
+      </c>
+      <c r="B16">
+        <v>1.3018000000000001</v>
+      </c>
+      <c r="C16">
+        <v>0.20030000000000001</v>
+      </c>
+      <c r="D16">
+        <v>0.88100000000000001</v>
+      </c>
+      <c r="E16">
+        <v>1.7225999999999999</v>
+      </c>
+      <c r="F16">
+        <f t="shared" si="1"/>
+        <v>0.42079999999999984</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>325</v>
+      </c>
+      <c r="B18">
+        <v>1.1759999999999999</v>
+      </c>
+      <c r="C18">
+        <v>0.23799999999999999</v>
+      </c>
+      <c r="D18">
+        <v>0.68859999999999999</v>
+      </c>
+      <c r="E18">
+        <v>1.6634</v>
+      </c>
+      <c r="F18">
+        <f>E18-B18</f>
+        <v>0.48740000000000006</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>326</v>
+      </c>
+      <c r="B19">
+        <v>1.361</v>
+      </c>
+      <c r="C19">
+        <v>0.1757</v>
+      </c>
+      <c r="D19">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>1.7222</v>
+      </c>
+      <c r="F19">
+        <f>E19-B19</f>
+        <v>0.36119999999999997</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
       </c>
     </row>
   </sheetData>
@@ -37133,7 +39638,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{58727C71-4C3B-4DE8-9714-FB21B562A65A}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView topLeftCell="C12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+    <sheetView topLeftCell="H1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
       <selection activeCell="B6" sqref="B6:X6"/>
     </sheetView>
   </sheetViews>
@@ -38515,7 +41020,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4DF2ECAC-65D2-4A41-A641-8078D11BDBA6}">
   <dimension ref="A1:X16"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="X39" sqref="X39"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
vault backup: 2025-07-20 21:31:28
</commit_message>
<xml_diff>
--- a/Economics/Dissertation/Dissertation Presentation Sheets.xlsx
+++ b/Economics/Dissertation/Dissertation Presentation Sheets.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\University Documents\Notes\PPE\Shared Notes\Economics\Dissertation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2BF1B8E-2E63-4FA4-A2DE-34702E63FFE1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{6B28940F-6CCE-4134-AE71-D2B2D380A4D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" firstSheet="12" activeTab="15" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
+    <workbookView xWindow="31440" yWindow="2640" windowWidth="21600" windowHeight="11385" firstSheet="12" activeTab="15" xr2:uid="{5E7F3A71-BFC8-4E5A-9B94-DE35856B8CBC}"/>
   </bookViews>
   <sheets>
     <sheet name="Median Wage and Productivity" sheetId="1" r:id="rId1"/>
@@ -35,6 +35,7 @@
     <definedName name="_xlnm._FilterDatabase" localSheetId="10" hidden="1">'Output Price Deflators'!$F$1:$I$94</definedName>
   </definedNames>
   <calcPr calcId="191029" calcOnSave="0"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -55,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="583" uniqueCount="330">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="589" uniqueCount="334">
   <si>
     <t>Year</t>
   </si>
@@ -1049,6 +1050,18 @@
   <si>
     <t>Median Wage adj. CPI</t>
   </si>
+  <si>
+    <t>Post</t>
+  </si>
+  <si>
+    <t>Pre</t>
+  </si>
+  <si>
+    <t>SD</t>
+  </si>
+  <si>
+    <t>Error</t>
+  </si>
 </sst>
 </file>
 
@@ -2574,7 +2587,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3366,6 +3379,32 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1600" baseline="0"/>
+              <a:t>Employees' earnings over time across the income distribution.</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1600"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -3379,7 +3418,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1600" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -3391,7 +3430,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="en-GB"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -3410,7 +3449,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>10th percentile Indexed, 1997=100</c:v>
+                  <c:v>10th percentile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3601,7 +3640,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>30th percentile Indexed, 1997=100</c:v>
+                  <c:v>30th percentile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3789,7 +3828,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>50th percentile Indexed, 1997=100</c:v>
+                  <c:v>50th percentile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -3980,7 +4019,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>70th percentile Indexed, 1997=100</c:v>
+                  <c:v>70th percentile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4171,7 +4210,7 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>90th percentile Indexed, 1997=100</c:v>
+                  <c:v>90th percentile</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -4349,194 +4388,6 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000004-6423-4365-AC03-E10661752205}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:ser>
-          <c:idx val="9"/>
-          <c:order val="9"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Distributions and Productivity'!$A$30</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>OpH Index 1997=100</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent2"/>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="none"/>
-          </c:marker>
-          <c:cat>
-            <c:strRef>
-              <c:f>'Distributions and Productivity'!$B$1:$X$1</c:f>
-              <c:strCache>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>1997</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>1998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>1999</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>2000</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>2001</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>2002</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2003</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>2004</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>2005</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2006</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>2007</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>2008</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>2009</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>2010</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>2011</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>2012</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>2013</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>2014</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>2015</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2016</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>2017</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>2018</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>2019</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Distributions and Productivity'!$B$30:$X$30</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>100</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>102.89224530396781</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>105.22151153897393</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>110.11689607230856</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>111.95550939981267</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>114.24492211450895</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>117.3349258161599</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>119.05388346952415</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>121.5062201622256</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>123.6699599543396</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>126.42223712040463</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>125.72315108708702</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>122.786133586068</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>125.14436710263364</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>126.53838841351332</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>125.77824998745741</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>125.45270750400881</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>126.1136535895529</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>126.50842591402574</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>127.21991209652354</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>129.69831118789767</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>130.11789103027519</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>130.42245188085167</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000005-6423-4365-AC03-E10661752205}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -4569,7 +4420,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>20th percentile Indexed, 1997=100</c:v>
+                        <c:v>20th percentile</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -4777,7 +4628,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>40th percentile Indexed, 1997=100</c:v>
+                        <c:v>40th percentile</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -4985,7 +4836,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>60th percentile Indexed, 1997=100</c:v>
+                        <c:v>60th percentile</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -5193,7 +5044,7 @@
                     <c:strCache>
                       <c:ptCount val="1"/>
                       <c:pt idx="0">
-                        <c:v>80th percentile Indexed, 1997=100</c:v>
+                        <c:v>80th percentile</c:v>
                       </c:pt>
                     </c:strCache>
                   </c:strRef>
@@ -5383,6 +5234,214 @@
                 <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000009-6423-4365-AC03-E10661752205}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="9"/>
+                <c:order val="9"/>
+                <c:tx>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Distributions and Productivity'!$A$30</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="1"/>
+                      <c:pt idx="0">
+                        <c:v>OpH Index 1997=100</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent2"/>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="none"/>
+                </c:marker>
+                <c:cat>
+                  <c:strRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Distributions and Productivity'!$B$1:$X$1</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:strCache>
+                      <c:ptCount val="23"/>
+                      <c:pt idx="0">
+                        <c:v>1997</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>1998</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>1999</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>2000</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>2001</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>2002</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>2003</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>2004</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>2005</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>2006</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>2007</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>2008</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>2009</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>2010</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>2011</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>2012</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>2013</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>2014</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>2015</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>2016</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>2017</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>2018</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>2019</c:v>
+                      </c:pt>
+                    </c:strCache>
+                  </c:strRef>
+                </c:cat>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                      <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Distributions and Productivity'!$B$30:$X$30</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="23"/>
+                      <c:pt idx="0">
+                        <c:v>100</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>102.89224530396781</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>105.22151153897393</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>110.11689607230856</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>111.95550939981267</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>114.24492211450895</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>117.3349258161599</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>119.05388346952415</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>121.5062201622256</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>123.6699599543396</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>126.42223712040463</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>125.72315108708702</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>122.786133586068</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>125.14436710263364</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>126.53838841351332</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>125.77824998745741</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>125.45270750400881</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>126.1136535895529</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>126.50842591402574</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>127.21991209652354</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>129.69831118789767</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>130.11789103027519</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>130.42245188085167</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000005-6423-4365-AC03-E10661752205}"/>
                   </c:ext>
                 </c:extLst>
               </c15:ser>
@@ -5415,7 +5474,7 @@
           <a:effectLst/>
         </c:spPr>
         <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" wrap="square" anchor="ctr" anchorCtr="1"/>
           <a:lstStyle/>
           <a:p>
             <a:pPr>
@@ -5463,6 +5522,61 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200"/>
+                  <a:t>Index 1997=100</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1200" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -5507,7 +5621,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -5521,7 +5635,7 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+            <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
@@ -9971,20 +10085,22 @@
           <a:lstStyle/>
           <a:p>
             <a:pPr>
-              <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
                 <a:solidFill>
                   <a:schemeClr val="tx1">
                     <a:lumMod val="65000"/>
                     <a:lumOff val="35000"/>
                   </a:schemeClr>
                 </a:solidFill>
-                <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                <a:latin typeface="+mn-lt"/>
                 <a:ea typeface="+mn-ea"/>
                 <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
               </a:defRPr>
             </a:pPr>
             <a:r>
-              <a:rPr lang="en-GB" sz="2000"/>
+              <a:rPr lang="en-GB" sz="1800">
+                <a:latin typeface="+mn-lt"/>
+              </a:rPr>
               <a:t>Consumer and Producer Price Indices, 1997=100</a:t>
             </a:r>
           </a:p>
@@ -10003,14 +10119,14 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="2000" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1800" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
               <a:solidFill>
                 <a:schemeClr val="tx1">
                   <a:lumMod val="65000"/>
                   <a:lumOff val="35000"/>
                 </a:schemeClr>
               </a:solidFill>
-              <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+              <a:latin typeface="+mn-lt"/>
               <a:ea typeface="+mn-ea"/>
               <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
             </a:defRPr>
@@ -10041,19 +10157,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:srgbClr val="FFC000"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:srgbClr val="FFC000"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -10237,25 +10341,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent3">
-                  <a:lumMod val="60000"/>
-                  <a:lumOff val="40000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent3">
-                    <a:lumMod val="60000"/>
-                    <a:lumOff val="40000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -10433,19 +10519,7 @@
             <a:effectLst/>
           </c:spPr>
           <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4"/>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4"/>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
+            <c:symbol val="none"/>
           </c:marker>
           <c:cat>
             <c:numRef>
@@ -10618,22 +10692,6 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:dropLines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="35000"/>
-                  <a:lumOff val="65000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:prstDash val="dash"/>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:dropLines>
-        <c:marker val="1"/>
         <c:smooth val="0"/>
         <c:axId val="1436691455"/>
         <c:axId val="1436696735"/>
@@ -11143,13 +11201,15 @@
                         <a:lumOff val="35000"/>
                       </a:schemeClr>
                     </a:solidFill>
-                    <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                    <a:latin typeface="+mn-lt"/>
                     <a:ea typeface="+mn-ea"/>
                     <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                   </a:defRPr>
                 </a:pPr>
                 <a:r>
-                  <a:rPr lang="en-GB"/>
+                  <a:rPr lang="en-GB">
+                    <a:latin typeface="+mn-lt"/>
+                  </a:rPr>
                   <a:t>Index 1997=100</a:t>
                 </a:r>
               </a:p>
@@ -11175,7 +11235,7 @@
                       <a:lumOff val="35000"/>
                     </a:schemeClr>
                   </a:solidFill>
-                  <a:latin typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
+                  <a:latin typeface="+mn-lt"/>
                   <a:ea typeface="+mn-ea"/>
                   <a:cs typeface="Times New Roman" panose="02020603050405020304" pitchFamily="18" charset="0"/>
                 </a:defRPr>
@@ -11229,7 +11289,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="t"/>
+      <c:legendPos val="r"/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -12131,63 +12191,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:tx>
-        <c:rich>
-          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:r>
-              <a:rPr lang="en-US" baseline="0"/>
-              <a:t>Shares of Income</a:t>
-            </a:r>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:rich>
-      </c:tx>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -12197,7 +12201,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Labour Share (LHS)</c:v>
+            <c:v>Labour Share of Income</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -12411,127 +12415,6 @@
       <c:lineChart>
         <c:grouping val="standard"/>
         <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="1"/>
-          <c:order val="1"/>
-          <c:tx>
-            <c:v>Profit Share (RHS)</c:v>
-          </c:tx>
-          <c:spPr>
-            <a:ln w="28575" cap="rnd">
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:marker>
-            <c:symbol val="circle"/>
-            <c:size val="5"/>
-            <c:spPr>
-              <a:solidFill>
-                <a:schemeClr val="accent4">
-                  <a:lumMod val="75000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent4">
-                    <a:lumMod val="75000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-              </a:ln>
-              <a:effectLst/>
-            </c:spPr>
-          </c:marker>
-          <c:val>
-            <c:numRef>
-              <c:f>'Labour Share of Income'!$C$2:$C$24</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="23"/>
-                <c:pt idx="0">
-                  <c:v>44.659199999999998</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>44.298099999999998</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>42.042000000000002</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>40.999600000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>39.8887</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>40.704300000000003</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>41.1858</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>40.302500000000002</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>40.548000000000002</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>40.165399999999998</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>39.421700000000001</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>40.639400000000002</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>39.581299999999999</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>39.507899999999999</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>39.953899999999997</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>40.6815</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>40.5886</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>41.718800000000002</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>41.391599999999997</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>41.422899999999998</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>41.566000000000003</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>41.113599999999998</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>40.851199999999999</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:smooth val="0"/>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000003-F235-487A-BEAE-22871C4322E1}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
         <c:dLbls>
           <c:showLegendKey val="0"/>
           <c:showVal val="0"/>
@@ -12544,6 +12427,139 @@
         <c:smooth val="0"/>
         <c:axId val="1513622463"/>
         <c:axId val="1513621983"/>
+        <c:extLst>
+          <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+            <c15:filteredLineSeries>
+              <c15:ser>
+                <c:idx val="1"/>
+                <c:order val="1"/>
+                <c:tx>
+                  <c:v>Profit Share (RHS)</c:v>
+                </c:tx>
+                <c:spPr>
+                  <a:ln w="28575" cap="rnd">
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:round/>
+                  </a:ln>
+                  <a:effectLst/>
+                </c:spPr>
+                <c:marker>
+                  <c:symbol val="circle"/>
+                  <c:size val="5"/>
+                  <c:spPr>
+                    <a:solidFill>
+                      <a:schemeClr val="accent4">
+                        <a:lumMod val="75000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:ln w="9525">
+                      <a:solidFill>
+                        <a:schemeClr val="accent4">
+                          <a:lumMod val="75000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                    </a:ln>
+                    <a:effectLst/>
+                  </c:spPr>
+                </c:marker>
+                <c:val>
+                  <c:numRef>
+                    <c:extLst>
+                      <c:ext uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
+                        <c15:formulaRef>
+                          <c15:sqref>'Labour Share of Income'!$C$2:$C$24</c15:sqref>
+                        </c15:formulaRef>
+                      </c:ext>
+                    </c:extLst>
+                    <c:numCache>
+                      <c:formatCode>General</c:formatCode>
+                      <c:ptCount val="23"/>
+                      <c:pt idx="0">
+                        <c:v>44.659199999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="1">
+                        <c:v>44.298099999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="2">
+                        <c:v>42.042000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="3">
+                        <c:v>40.999600000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="4">
+                        <c:v>39.8887</c:v>
+                      </c:pt>
+                      <c:pt idx="5">
+                        <c:v>40.704300000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="6">
+                        <c:v>41.1858</c:v>
+                      </c:pt>
+                      <c:pt idx="7">
+                        <c:v>40.302500000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="8">
+                        <c:v>40.548000000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="9">
+                        <c:v>40.165399999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="10">
+                        <c:v>39.421700000000001</c:v>
+                      </c:pt>
+                      <c:pt idx="11">
+                        <c:v>40.639400000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="12">
+                        <c:v>39.581299999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="13">
+                        <c:v>39.507899999999999</c:v>
+                      </c:pt>
+                      <c:pt idx="14">
+                        <c:v>39.953899999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="15">
+                        <c:v>40.6815</c:v>
+                      </c:pt>
+                      <c:pt idx="16">
+                        <c:v>40.5886</c:v>
+                      </c:pt>
+                      <c:pt idx="17">
+                        <c:v>41.718800000000002</c:v>
+                      </c:pt>
+                      <c:pt idx="18">
+                        <c:v>41.391599999999997</c:v>
+                      </c:pt>
+                      <c:pt idx="19">
+                        <c:v>41.422899999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="20">
+                        <c:v>41.566000000000003</c:v>
+                      </c:pt>
+                      <c:pt idx="21">
+                        <c:v>41.113599999999998</c:v>
+                      </c:pt>
+                      <c:pt idx="22">
+                        <c:v>40.851199999999999</c:v>
+                      </c:pt>
+                    </c:numCache>
+                  </c:numRef>
+                </c:val>
+                <c:smooth val="0"/>
+                <c:extLst>
+                  <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+                    <c16:uniqueId val="{00000003-F235-487A-BEAE-22871C4322E1}"/>
+                  </c:ext>
+                </c:extLst>
+              </c15:ser>
+            </c15:filteredLineSeries>
+          </c:ext>
+        </c:extLst>
       </c:lineChart>
       <c:catAx>
         <c:axId val="368218511"/>
@@ -12714,99 +12730,12 @@
           <c:orientation val="minMax"/>
           <c:min val="38"/>
         </c:scaling>
-        <c:delete val="0"/>
+        <c:delete val="1"/>
         <c:axPos val="r"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="en-GB"/>
-                  <a:t>Profit Share of Income</a:t>
-                </a:r>
-                <a:r>
-                  <a:rPr lang="en-GB" baseline="0"/>
-                  <a:t> (%)</a:t>
-                </a:r>
-                <a:endParaRPr lang="en-GB"/>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-GB"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="out"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-US"/>
-          </a:p>
-        </c:txPr>
         <c:crossAx val="1513622463"/>
         <c:crosses val="max"/>
         <c:crossBetween val="between"/>
@@ -18003,6 +17932,1590 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart27.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Productivity effect on wage growth across the income distribution</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-GB" sz="1400"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Real RegressionII Results'!$F$16:$F$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>0.38374091437332436</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.26501444362798643</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.25653398143189088</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.29893629241236869</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.29469606131432091</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.31589721680455979</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.33497825674577486</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.30953687015748815</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.29681617686334483</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Real RegressionII Results'!$F$16:$F$24</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>0.38374091437332436</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.26501444362798643</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.25653398143189088</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.29893629241236869</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.29469606131432091</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.31589721680455979</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.33497825674577486</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.30953687015748815</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.29681617686334483</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln w="6350"/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$B$16:$B$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.877</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.83799999999999997</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.97099999999999997</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.022</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0469999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.129</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2290000000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.292</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.3740000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-F7CA-4C18-B8B1-9D77E66B4B55}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="12700" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$G$16:$G$24</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-F7CA-4C18-B8B1-9D77E66B4B55}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1044153904"/>
+        <c:axId val="1044145744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1044153904"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1050" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1050" b="0"/>
+                  <a:t>Decile</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044145744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1044145744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="1.9"/>
+          <c:min val="0.4"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1100" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1100" b="0"/>
+                  <a:t>Productivity Elasticity (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1044153904"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart28.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Productivity effect on wage growth across the income distribution Pre-2008</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.340041357186094E-2"/>
+          <c:y val="9.4000695681869181E-2"/>
+          <c:w val="0.88882174103237099"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.60899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.3717E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.15124070000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.29240640000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1177039</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.6312500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41357450000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-3693-41E8-9E7F-D29B02752528}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln>
+                <a:noFill/>
+              </a:ln>
+            </c:spPr>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Real RegressionII Results'!$G$27:$G$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>1.1173606815940731</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.76473055479868035</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.72186817874406439</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.84400676345400139</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.84168587296248498</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.84202657553121296</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.89721381930696964</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.77260084773976678</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.81874028639850915</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Real RegressionII Results'!$G$27:$G$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>1.1173606815940731</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.76473055479868035</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.72186817874406439</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.84400676345400139</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.84168587296248498</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.84202657553121296</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.89721381930696964</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.77260084773976678</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.81874028639850915</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln w="6350"/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$E$27:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50442880000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.893621</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.075582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.303226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2352730000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2364250000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88039440000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-3693-41E8-9E7F-D29B02752528}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="6350">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$H$27:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000004-3693-41E8-9E7F-D29B02752528}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="6350">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$I$27:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000005-3693-41E8-9E7F-D29B02752528}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="1218392256"/>
+        <c:axId val="1218397536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1218392256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0"/>
+                  <a:t>Decile</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.48306762432495848"/>
+              <c:y val="0.92748266419620762"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218397536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1218397536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0"/>
+                  <a:t>Productivity Elasticity (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218392256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart29.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-GB" sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:sysClr val="windowText" lastClr="000000">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:sysClr>
+                </a:solidFill>
+              </a:rPr>
+              <a:t>Productivity effect on wage growth across the income distribution Pre-2008</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="8.340041357186094E-2"/>
+          <c:y val="9.4000695681869181E-2"/>
+          <c:w val="0.88882174103237099"/>
+          <c:h val="0.77736111111111106"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="diamond"/>
+            <c:size val="5"/>
+          </c:marker>
+          <c:errBars>
+            <c:errDir val="y"/>
+            <c:errBarType val="both"/>
+            <c:errValType val="cust"/>
+            <c:noEndCap val="0"/>
+            <c:plus>
+              <c:numRef>
+                <c:f>'Real RegressionII Results'!$D$27:$D$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>1.1978652851984986</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.84380598851150879</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.7831908249071412</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.91213519254099973</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.89044853059003437</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.88595155349899979</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.92758087035030357</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.81181895717716568</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.8744486545762159</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:plus>
+            <c:minus>
+              <c:numRef>
+                <c:f>'Real RegressionII Results'!$D$27:$D$35</c:f>
+                <c:numCache>
+                  <c:formatCode>General</c:formatCode>
+                  <c:ptCount val="9"/>
+                  <c:pt idx="0">
+                    <c:v>1.1978652851984986</c:v>
+                  </c:pt>
+                  <c:pt idx="1">
+                    <c:v>0.84380598851150879</c:v>
+                  </c:pt>
+                  <c:pt idx="2">
+                    <c:v>0.7831908249071412</c:v>
+                  </c:pt>
+                  <c:pt idx="3">
+                    <c:v>0.91213519254099973</c:v>
+                  </c:pt>
+                  <c:pt idx="4">
+                    <c:v>0.89044853059003437</c:v>
+                  </c:pt>
+                  <c:pt idx="5">
+                    <c:v>0.88595155349899979</c:v>
+                  </c:pt>
+                  <c:pt idx="6">
+                    <c:v>0.92758087035030357</c:v>
+                  </c:pt>
+                  <c:pt idx="7">
+                    <c:v>0.81181895717716568</c:v>
+                  </c:pt>
+                  <c:pt idx="8">
+                    <c:v>0.8744486545762159</c:v>
+                  </c:pt>
+                </c:numCache>
+              </c:numRef>
+            </c:minus>
+            <c:spPr>
+              <a:ln w="6350"/>
+            </c:spPr>
+          </c:errBars>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$B$27:$B$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.60899999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.28799999999999998</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>-3.3717E-3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>-0.15124070000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>-0.20399999999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>-0.29240640000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>-0.1177039</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>-5.6312500000000001E-2</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.41357450000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-DADD-43AB-9C5B-516200212949}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="1"/>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$E$27:$E$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0.246</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.50442880000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.893621</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.075582</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.147</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.303226</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2352730000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.2364250000000001</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0.88039440000000002</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-DADD-43AB-9C5B-516200212949}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:spPr>
+            <a:ln w="6350">
+              <a:solidFill>
+                <a:schemeClr val="accent6"/>
+              </a:solidFill>
+              <a:prstDash val="sysDash"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$H$27:$H$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-DADD-43AB-9C5B-516200212949}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:spPr>
+            <a:ln w="6350">
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:prstDash val="sysDot"/>
+            </a:ln>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:val>
+            <c:numRef>
+              <c:f>'Real RegressionII Results'!$I$27:$I$35</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>0</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-DADD-43AB-9C5B-516200212949}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:marker val="1"/>
+        <c:smooth val="0"/>
+        <c:axId val="1218392256"/>
+        <c:axId val="1218397536"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="1218392256"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1200" b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" sz="1200" b="0"/>
+                  <a:t>Decile</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.48306762432495848"/>
+              <c:y val="0.92748266419620762"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="low"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="t" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218397536"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1218397536"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr b="0"/>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-GB" b="0"/>
+                  <a:t>Productivity Elasticity (%)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1218392256"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+    <c:extLst/>
+  </c:chart>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
@@ -24242,7 +25755,7 @@
                 </c:marker>
                 <c:cat>
                   <c:strRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Mean Median and Prod GDP'!$B$1:$X$1</c15:sqref>
@@ -24325,7 +25838,7 @@
                 </c:cat>
                 <c:val>
                   <c:numRef>
-                    <c:extLst>
+                    <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                       <c:ext xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart" uri="{02D57815-91ED-43cb-92C2-25804820EDAC}">
                         <c15:formulaRef>
                           <c15:sqref>'Mean Median and Prod GDP'!$B$11:$X$11</c15:sqref>
@@ -24408,7 +25921,7 @@
                   </c:numRef>
                 </c:val>
                 <c:smooth val="0"/>
-                <c:extLst>
+                <c:extLst xmlns:c15="http://schemas.microsoft.com/office/drawing/2012/chart">
                   <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
                     <c16:uniqueId val="{00000002-454E-4F28-A4B2-1A58C737A23E}"/>
                   </c:ext>
@@ -36824,8 +38337,8 @@
       <xdr:rowOff>114300</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>976314</xdr:colOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1085850</xdr:colOff>
       <xdr:row>33</xdr:row>
       <xdr:rowOff>14289</xdr:rowOff>
     </xdr:to>
@@ -36902,16 +38415,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>3</xdr:col>
-      <xdr:colOff>109536</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>142876</xdr:rowOff>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>14286</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>9526</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>12</xdr:col>
-      <xdr:colOff>561975</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>152400</xdr:rowOff>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>466725</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37219,16 +38732,16 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor>
     <xdr:from>
-      <xdr:col>8</xdr:col>
-      <xdr:colOff>604628</xdr:colOff>
-      <xdr:row>20</xdr:row>
-      <xdr:rowOff>165653</xdr:rowOff>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>57976</xdr:colOff>
+      <xdr:row>21</xdr:row>
+      <xdr:rowOff>115958</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>15</xdr:col>
-      <xdr:colOff>505237</xdr:colOff>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>571498</xdr:colOff>
       <xdr:row>38</xdr:row>
-      <xdr:rowOff>1</xdr:rowOff>
+      <xdr:rowOff>140806</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -37250,6 +38763,116 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>10</xdr:col>
+      <xdr:colOff>509379</xdr:colOff>
+      <xdr:row>8</xdr:row>
+      <xdr:rowOff>173937</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>117336</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>21540</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{1CDB5C8C-7BDD-BFC8-24AF-A96B702174A0}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId3"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>467964</xdr:colOff>
+      <xdr:row>14</xdr:row>
+      <xdr:rowOff>168964</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>190497</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>16566</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="4" name="Chart 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E9901E43-B378-DD31-C0AA-09D61DAB4547}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId4"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>323022</xdr:colOff>
+      <xdr:row>28</xdr:row>
+      <xdr:rowOff>8282</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>45555</xdr:colOff>
+      <xdr:row>46</xdr:row>
+      <xdr:rowOff>46384</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="9" name="Chart 8">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{69ACEB95-FF9B-4125-A86A-D4976EDB403B}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId5"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -37539,15 +39162,15 @@
   <xdr:twoCellAnchor>
     <xdr:from>
       <xdr:col>24</xdr:col>
-      <xdr:colOff>0</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:colOff>561975</xdr:colOff>
+      <xdr:row>2</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>36</xdr:col>
-      <xdr:colOff>214314</xdr:colOff>
-      <xdr:row>18</xdr:row>
-      <xdr:rowOff>166689</xdr:rowOff>
+      <xdr:col>37</xdr:col>
+      <xdr:colOff>166689</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
@@ -39802,7 +41425,7 @@
   <dimension ref="A1:P26"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="R13" sqref="R13"/>
+      <selection activeCell="AM18" sqref="AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -44260,7 +45883,7 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G31" sqref="G31"/>
+      <selection activeCell="O11" sqref="O11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45422,7 +47045,7 @@
         <v>1.6857</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F6" si="0">E3-B3</f>
+        <f>E3-B3</f>
         <v>0.6371</v>
       </c>
       <c r="G3">
@@ -45446,7 +47069,7 @@
         <v>1.8425</v>
       </c>
       <c r="F4">
-        <f t="shared" si="0"/>
+        <f>E4-B4</f>
         <v>0.71250000000000013</v>
       </c>
       <c r="G4">
@@ -45470,7 +47093,7 @@
         <v>2.0049999999999999</v>
       </c>
       <c r="F5">
-        <f t="shared" si="0"/>
+        <f>E5-B5</f>
         <v>0.78959999999999986</v>
       </c>
       <c r="G5">
@@ -45494,7 +47117,7 @@
         <v>2.117</v>
       </c>
       <c r="F6">
-        <f t="shared" si="0"/>
+        <f>E6-B6</f>
         <v>0.78200000000000003</v>
       </c>
       <c r="G6">
@@ -45543,7 +47166,7 @@
         <v>1.1476999999999999</v>
       </c>
       <c r="F9">
-        <f t="shared" ref="F9:F16" si="1">E9-B9</f>
+        <f t="shared" ref="F9:F16" si="0">E9-B9</f>
         <v>0.3708999999999999</v>
       </c>
       <c r="G9">
@@ -45552,7 +47175,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="23">
-        <f t="shared" ref="A10:A16" si="2">A9+10</f>
+        <f t="shared" ref="A10:A16" si="1">A9+10</f>
         <v>30</v>
       </c>
       <c r="B10">
@@ -45568,7 +47191,7 @@
         <v>1.2750999999999999</v>
       </c>
       <c r="F10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.3647999999999999</v>
       </c>
       <c r="G10">
@@ -45577,7 +47200,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>40</v>
       </c>
       <c r="B11">
@@ -45593,7 +47216,7 @@
         <v>1.3499000000000001</v>
       </c>
       <c r="F11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.38510000000000011</v>
       </c>
       <c r="G11">
@@ -45602,7 +47225,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>50</v>
       </c>
       <c r="B12">
@@ -45618,7 +47241,7 @@
         <v>1.3829</v>
       </c>
       <c r="F12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.39890000000000003</v>
       </c>
       <c r="G12">
@@ -45627,7 +47250,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>60</v>
       </c>
       <c r="B13">
@@ -45643,7 +47266,7 @@
         <v>1.4732000000000001</v>
       </c>
       <c r="F13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.40470000000000006</v>
       </c>
       <c r="G13">
@@ -45652,7 +47275,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>70</v>
       </c>
       <c r="B14">
@@ -45668,7 +47291,7 @@
         <v>1.5802</v>
       </c>
       <c r="F14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.41030000000000011</v>
       </c>
       <c r="G14">
@@ -45677,7 +47300,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>80</v>
       </c>
       <c r="B15">
@@ -45693,7 +47316,7 @@
         <v>1.64</v>
       </c>
       <c r="F15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.41449999999999987</v>
       </c>
       <c r="G15">
@@ -45702,7 +47325,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="23">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>90</v>
       </c>
       <c r="B16">
@@ -45718,7 +47341,7 @@
         <v>1.7225999999999999</v>
       </c>
       <c r="F16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.42079999999999984</v>
       </c>
       <c r="G16">
@@ -45784,10 +47407,10 @@
 
 <file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{511D93AE-C435-412E-812E-E16DB06983DD}">
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:I35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="I27" sqref="I27"/>
+    <sheetView tabSelected="1" topLeftCell="A22" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="D43" sqref="D43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -45796,7 +47419,7 @@
     <col min="2" max="2" width="11.5703125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="24" t="s">
         <v>320</v>
       </c>
@@ -45815,7 +47438,7 @@
       </c>
       <c r="G1" s="24"/>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>10</v>
       </c>
@@ -45832,14 +47455,18 @@
         <v>0.98919999999999997</v>
       </c>
       <c r="F2">
-        <f>E2-B2</f>
+        <f t="shared" ref="F2:F10" si="0">E2-B2</f>
         <v>0.34309999999999996</v>
       </c>
       <c r="G2">
         <v>1</v>
       </c>
+      <c r="H2">
+        <f>F2/C2</f>
+        <v>2.1205191594561184</v>
+      </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3">
         <f>A2+10</f>
         <v>20</v>
@@ -45857,16 +47484,20 @@
         <v>1.0298</v>
       </c>
       <c r="F3">
-        <f t="shared" ref="F3:F13" si="0">E3-B3</f>
+        <f t="shared" si="0"/>
         <v>0.31780000000000008</v>
       </c>
       <c r="G3">
         <v>1</v>
       </c>
+      <c r="H3">
+        <f t="shared" ref="H3:H10" si="1">F3/C3</f>
+        <v>2.120080053368913</v>
+      </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4">
-        <f t="shared" ref="A4:A10" si="1">A3+10</f>
+        <f t="shared" ref="A4:A10" si="2">A3+10</f>
         <v>30</v>
       </c>
       <c r="B4">
@@ -45888,10 +47519,14 @@
       <c r="G4">
         <v>1</v>
       </c>
+      <c r="H4">
+        <f t="shared" si="1"/>
+        <v>2.120306513409961</v>
+      </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>40</v>
       </c>
       <c r="B5">
@@ -45913,10 +47548,14 @@
       <c r="G5">
         <v>1</v>
       </c>
+      <c r="H5">
+        <f t="shared" si="1"/>
+        <v>2.1200324412003249</v>
+      </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>50</v>
       </c>
       <c r="B6">
@@ -45938,10 +47577,14 @@
       <c r="G6">
         <v>1</v>
       </c>
+      <c r="H6">
+        <f t="shared" si="1"/>
+        <v>2.1198347107438011</v>
+      </c>
     </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>60</v>
       </c>
       <c r="B7">
@@ -45963,10 +47606,14 @@
       <c r="G7">
         <v>1</v>
       </c>
+      <c r="H7">
+        <f t="shared" si="1"/>
+        <v>2.120539254559874</v>
+      </c>
     </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>70</v>
       </c>
       <c r="B8">
@@ -45988,8 +47635,12 @@
       <c r="G8">
         <v>1</v>
       </c>
+      <c r="H8">
+        <f t="shared" si="1"/>
+        <v>2.1196787148594378</v>
+      </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9">
         <f>A8+10</f>
         <v>80</v>
@@ -46013,10 +47664,14 @@
       <c r="G9">
         <v>1</v>
       </c>
+      <c r="H9">
+        <f t="shared" si="1"/>
+        <v>2.1199690402476783</v>
+      </c>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="2"/>
         <v>90</v>
       </c>
       <c r="B10">
@@ -46038,8 +47693,18 @@
       <c r="G10">
         <v>1</v>
       </c>
+      <c r="H10">
+        <f t="shared" si="1"/>
+        <v>2.1200800533689117</v>
+      </c>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="H11">
+        <f>AVERAGE(H2:H10)</f>
+        <v>2.1201155490238914</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>325</v>
       </c>
@@ -46056,14 +47721,14 @@
         <v>1.5243119999999999</v>
       </c>
       <c r="F12">
-        <f t="shared" si="0"/>
+        <f>E12-B12</f>
         <v>0.2667799999999998</v>
       </c>
       <c r="G12">
         <v>1</v>
       </c>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>326</v>
       </c>
@@ -46080,11 +47745,482 @@
         <v>2.0556009999999998</v>
       </c>
       <c r="F13">
-        <f t="shared" si="0"/>
+        <f>E13-B13</f>
         <v>0.25485599999999975</v>
       </c>
       <c r="G13">
         <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G15">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A16">
+        <v>10</v>
+      </c>
+      <c r="B16">
+        <v>0.877</v>
+      </c>
+      <c r="C16">
+        <v>0.18099999999999999</v>
+      </c>
+      <c r="F16">
+        <f>C16*$H$11</f>
+        <v>0.38374091437332436</v>
+      </c>
+      <c r="G16">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A17">
+        <v>20</v>
+      </c>
+      <c r="B17">
+        <v>0.83799999999999997</v>
+      </c>
+      <c r="C17">
+        <v>0.125</v>
+      </c>
+      <c r="F17">
+        <f t="shared" ref="F17:F24" si="3">C17*$H$11</f>
+        <v>0.26501444362798643</v>
+      </c>
+      <c r="G17">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A18">
+        <v>30</v>
+      </c>
+      <c r="B18">
+        <v>0.97099999999999997</v>
+      </c>
+      <c r="C18">
+        <v>0.121</v>
+      </c>
+      <c r="F18">
+        <f t="shared" si="3"/>
+        <v>0.25653398143189088</v>
+      </c>
+      <c r="G18">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A19">
+        <v>40</v>
+      </c>
+      <c r="B19">
+        <v>1.022</v>
+      </c>
+      <c r="C19">
+        <v>0.14099999999999999</v>
+      </c>
+      <c r="F19">
+        <f t="shared" si="3"/>
+        <v>0.29893629241236869</v>
+      </c>
+      <c r="G19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A20">
+        <v>50</v>
+      </c>
+      <c r="B20">
+        <v>1.0469999999999999</v>
+      </c>
+      <c r="C20">
+        <v>0.13900000000000001</v>
+      </c>
+      <c r="F20">
+        <f t="shared" si="3"/>
+        <v>0.29469606131432091</v>
+      </c>
+      <c r="G20">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A21">
+        <v>60</v>
+      </c>
+      <c r="B21">
+        <v>1.129</v>
+      </c>
+      <c r="C21">
+        <v>0.14899999999999999</v>
+      </c>
+      <c r="F21">
+        <f t="shared" si="3"/>
+        <v>0.31589721680455979</v>
+      </c>
+      <c r="G21">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A22">
+        <v>70</v>
+      </c>
+      <c r="B22">
+        <v>1.2290000000000001</v>
+      </c>
+      <c r="C22">
+        <v>0.158</v>
+      </c>
+      <c r="F22">
+        <f t="shared" si="3"/>
+        <v>0.33497825674577486</v>
+      </c>
+      <c r="G22">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A23">
+        <v>80</v>
+      </c>
+      <c r="B23">
+        <v>1.292</v>
+      </c>
+      <c r="C23">
+        <v>0.14599999999999999</v>
+      </c>
+      <c r="F23">
+        <f t="shared" si="3"/>
+        <v>0.30953687015748815</v>
+      </c>
+      <c r="G23">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A24">
+        <v>90</v>
+      </c>
+      <c r="B24">
+        <v>1.3740000000000001</v>
+      </c>
+      <c r="C24">
+        <v>0.14000000000000001</v>
+      </c>
+      <c r="F24">
+        <f t="shared" si="3"/>
+        <v>0.29681617686334483</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="B26" t="s">
+        <v>330</v>
+      </c>
+      <c r="C26" t="s">
+        <v>332</v>
+      </c>
+      <c r="D26" t="s">
+        <v>333</v>
+      </c>
+      <c r="E26" t="s">
+        <v>331</v>
+      </c>
+      <c r="F26" t="s">
+        <v>332</v>
+      </c>
+      <c r="G26" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A27">
+        <v>10</v>
+      </c>
+      <c r="B27">
+        <v>0.60899999999999999</v>
+      </c>
+      <c r="C27">
+        <v>0.56499999999999995</v>
+      </c>
+      <c r="D27">
+        <f>C27*$H$11</f>
+        <v>1.1978652851984986</v>
+      </c>
+      <c r="E27">
+        <v>0.246</v>
+      </c>
+      <c r="F27">
+        <v>0.52702819999999995</v>
+      </c>
+      <c r="G27">
+        <f>F27*$H$11</f>
+        <v>1.1173606815940731</v>
+      </c>
+      <c r="H27">
+        <v>1</v>
+      </c>
+      <c r="I27">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A28">
+        <v>20</v>
+      </c>
+      <c r="B28">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="C28">
+        <v>0.39800000000000002</v>
+      </c>
+      <c r="D28">
+        <f t="shared" ref="D28:D35" si="4">C28*$H$11</f>
+        <v>0.84380598851150879</v>
+      </c>
+      <c r="E28">
+        <v>0.50442880000000001</v>
+      </c>
+      <c r="F28">
+        <v>0.36070229999999998</v>
+      </c>
+      <c r="G28">
+        <f t="shared" ref="G28:G35" si="5">F28*$H$11</f>
+        <v>0.76473055479868035</v>
+      </c>
+      <c r="H28">
+        <v>1</v>
+      </c>
+      <c r="I28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A29">
+        <v>30</v>
+      </c>
+      <c r="B29">
+        <v>-3.3717E-3</v>
+      </c>
+      <c r="C29">
+        <v>0.3694095</v>
+      </c>
+      <c r="D29">
+        <f t="shared" si="4"/>
+        <v>0.7831908249071412</v>
+      </c>
+      <c r="E29">
+        <v>0.893621</v>
+      </c>
+      <c r="F29">
+        <v>0.34048529999999999</v>
+      </c>
+      <c r="G29">
+        <f t="shared" si="5"/>
+        <v>0.72186817874406439</v>
+      </c>
+      <c r="H29">
+        <v>1</v>
+      </c>
+      <c r="I29">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A30">
+        <v>40</v>
+      </c>
+      <c r="B30">
+        <v>-0.15124070000000001</v>
+      </c>
+      <c r="C30">
+        <v>0.43022899999999997</v>
+      </c>
+      <c r="D30">
+        <f t="shared" si="4"/>
+        <v>0.91213519254099973</v>
+      </c>
+      <c r="E30">
+        <v>1.075582</v>
+      </c>
+      <c r="F30">
+        <v>0.39809470000000002</v>
+      </c>
+      <c r="G30">
+        <f t="shared" si="5"/>
+        <v>0.84400676345400139</v>
+      </c>
+      <c r="H30">
+        <v>1</v>
+      </c>
+      <c r="I30">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A31">
+        <v>50</v>
+      </c>
+      <c r="B31">
+        <v>-0.20399999999999999</v>
+      </c>
+      <c r="C31">
+        <v>0.42</v>
+      </c>
+      <c r="D31">
+        <f t="shared" si="4"/>
+        <v>0.89044853059003437</v>
+      </c>
+      <c r="E31">
+        <v>1.147</v>
+      </c>
+      <c r="F31">
+        <v>0.39700000000000002</v>
+      </c>
+      <c r="G31">
+        <f t="shared" si="5"/>
+        <v>0.84168587296248498</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+      <c r="I31">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A32">
+        <v>60</v>
+      </c>
+      <c r="B32">
+        <v>-0.29240640000000001</v>
+      </c>
+      <c r="C32">
+        <v>0.4178789</v>
+      </c>
+      <c r="D32">
+        <f t="shared" si="4"/>
+        <v>0.88595155349899979</v>
+      </c>
+      <c r="E32">
+        <v>1.303226</v>
+      </c>
+      <c r="F32">
+        <v>0.39716069999999998</v>
+      </c>
+      <c r="G32">
+        <f t="shared" si="5"/>
+        <v>0.84202657553121296</v>
+      </c>
+      <c r="H32">
+        <v>1</v>
+      </c>
+      <c r="I32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33">
+        <v>70</v>
+      </c>
+      <c r="B33">
+        <v>-0.1177039</v>
+      </c>
+      <c r="C33">
+        <v>0.43751430000000002</v>
+      </c>
+      <c r="D33">
+        <f t="shared" si="4"/>
+        <v>0.92758087035030357</v>
+      </c>
+      <c r="E33">
+        <v>1.2352730000000001</v>
+      </c>
+      <c r="F33">
+        <v>0.42319099999999998</v>
+      </c>
+      <c r="G33">
+        <f t="shared" si="5"/>
+        <v>0.89721381930696964</v>
+      </c>
+      <c r="H33">
+        <v>1</v>
+      </c>
+      <c r="I33">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34">
+        <v>80</v>
+      </c>
+      <c r="B34">
+        <v>-5.6312500000000001E-2</v>
+      </c>
+      <c r="C34">
+        <v>0.38291259999999999</v>
+      </c>
+      <c r="D34">
+        <f t="shared" si="4"/>
+        <v>0.81181895717716568</v>
+      </c>
+      <c r="E34">
+        <v>1.2364250000000001</v>
+      </c>
+      <c r="F34">
+        <v>0.36441449999999997</v>
+      </c>
+      <c r="G34">
+        <f t="shared" si="5"/>
+        <v>0.77260084773976678</v>
+      </c>
+      <c r="H34">
+        <v>1</v>
+      </c>
+      <c r="I34">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35">
+        <v>90</v>
+      </c>
+      <c r="B35">
+        <v>0.41357450000000001</v>
+      </c>
+      <c r="C35">
+        <v>0.41245330000000002</v>
+      </c>
+      <c r="D35">
+        <f t="shared" si="4"/>
+        <v>0.8744486545762159</v>
+      </c>
+      <c r="E35">
+        <v>0.88039440000000002</v>
+      </c>
+      <c r="F35">
+        <v>0.3861772</v>
+      </c>
+      <c r="G35">
+        <f t="shared" si="5"/>
+        <v>0.81874028639850915</v>
+      </c>
+      <c r="H35">
+        <v>1</v>
+      </c>
+      <c r="I35">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -50911,10 +53047,10 @@
   <dimension ref="A1:X39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="B28" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="Q13" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="B12" sqref="B12:X20"/>
+      <selection pane="bottomRight" activeCell="AM18" sqref="AM18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -52628,10 +54764,10 @@
         <v>26.771799628942485</v>
       </c>
     </row>
-    <row r="21" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="str">
-        <f>A2 &amp; " Indexed, 1997=100"</f>
-        <v>10th percentile Indexed, 1997=100</v>
+        <f>A2</f>
+        <v>10th percentile</v>
       </c>
       <c r="B21">
         <f t="shared" ref="B21:B29" si="5">B12*100/$B12</f>
@@ -52726,10 +54862,10 @@
         <v>142.51505899424907</v>
       </c>
     </row>
-    <row r="22" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="str">
-        <f t="shared" ref="A22:A29" si="7">A3 &amp; " Indexed, 1997=100"</f>
-        <v>20th percentile Indexed, 1997=100</v>
+        <f t="shared" ref="A22:A29" si="7">A3</f>
+        <v>20th percentile</v>
       </c>
       <c r="B22">
         <f t="shared" si="5"/>
@@ -52824,10 +54960,10 @@
         <v>130.33962294723366</v>
       </c>
     </row>
-    <row r="23" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>30th percentile Indexed, 1997=100</v>
+        <v>30th percentile</v>
       </c>
       <c r="B23">
         <f t="shared" si="5"/>
@@ -52922,10 +55058,10 @@
         <v>124.33223544780529</v>
       </c>
     </row>
-    <row r="24" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>40th percentile Indexed, 1997=100</v>
+        <v>40th percentile</v>
       </c>
       <c r="B24">
         <f t="shared" si="5"/>
@@ -53020,10 +55156,10 @@
         <v>122.74797096807333</v>
       </c>
     </row>
-    <row r="25" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>50th percentile Indexed, 1997=100</v>
+        <v>50th percentile</v>
       </c>
       <c r="B25">
         <f t="shared" si="5"/>
@@ -53118,10 +55254,10 @@
         <v>122.1456256412813</v>
       </c>
     </row>
-    <row r="26" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>60th percentile Indexed, 1997=100</v>
+        <v>60th percentile</v>
       </c>
       <c r="B26">
         <f t="shared" si="5"/>
@@ -53216,10 +55352,10 @@
         <v>122.32176630581621</v>
       </c>
     </row>
-    <row r="27" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>70th percentile Indexed, 1997=100</v>
+        <v>70th percentile</v>
       </c>
       <c r="B27">
         <f t="shared" si="5"/>
@@ -53314,10 +55450,10 @@
         <v>122.95684306865708</v>
       </c>
     </row>
-    <row r="28" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>80th percentile Indexed, 1997=100</v>
+        <v>80th percentile</v>
       </c>
       <c r="B28">
         <f t="shared" si="5"/>
@@ -53412,10 +55548,10 @@
         <v>121.99618232846467</v>
       </c>
     </row>
-    <row r="29" spans="1:24" ht="30" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="str">
         <f t="shared" si="7"/>
-        <v>90th percentile Indexed, 1997=100</v>
+        <v>90th percentile</v>
       </c>
       <c r="B29">
         <f t="shared" si="5"/>

</xml_diff>